<commit_message>
last corrections / testing
</commit_message>
<xml_diff>
--- a/desarrollo/the-vault/gestion/sprints_del_proyecto/TVT-SP02.xlsx
+++ b/desarrollo/the-vault/gestion/sprints_del_proyecto/TVT-SP02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssarm\Desktop\The-Vault\desarrollo\the-vault\gestion\sprints_del_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FC3663-37FA-4222-B685-69D8E0FFA2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61C24BC-BDC5-4C7F-9615-EE2BC1FA3F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -217,22 +217,10 @@
     <t>Sketches de interfaz de usuario</t>
   </si>
   <si>
-    <t>Interfaz de usuario</t>
-  </si>
-  <si>
-    <t>TVT-SKETCH.pdf</t>
-  </si>
-  <si>
     <t>Sarmiento/Diseñadora UX, Contreras/Diseñadora web, Aranda/Diseñador web</t>
   </si>
   <si>
-    <t>Esquema para organizar la base de datos</t>
-  </si>
-  <si>
     <t>Diagrama ER</t>
-  </si>
-  <si>
-    <t>TVT-BD.pdf</t>
   </si>
   <si>
     <t>Equipo backend</t>
@@ -298,9 +286,6 @@
     <t>Desarrollo de plan de prueba</t>
   </si>
   <si>
-    <t>Planificación de pruebas</t>
-  </si>
-  <si>
     <t>TVT-PDP.docx</t>
   </si>
   <si>
@@ -320,9 +305,6 @@
   </si>
   <si>
     <t>Documentación de resultados</t>
-  </si>
-  <si>
-    <t>Documento de los resultados y las modificaciones</t>
   </si>
   <si>
     <t>TVT-RDP.docx</t>
@@ -350,6 +332,24 @@
   </si>
   <si>
     <t>Semana 15</t>
+  </si>
+  <si>
+    <t>TVT-EBD.pdf</t>
+  </si>
+  <si>
+    <t>Esquema para la base de datos</t>
+  </si>
+  <si>
+    <t>TVT-IDU.pdf</t>
+  </si>
+  <si>
+    <t>Interfaz diseñada para el usuario</t>
+  </si>
+  <si>
+    <t>Planificación documentada de pruebas</t>
+  </si>
+  <si>
+    <t>Resultados documentados de las pruebas</t>
   </si>
 </sst>
 </file>
@@ -1329,33 +1329,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1388,6 +1361,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1607,7 +1607,7 @@
   <dimension ref="A1:AN1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1638,16 +1638,16 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="107"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="118"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
@@ -1715,11 +1715,11 @@
       <c r="R2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="115" t="s">
+      <c r="S2" s="102" t="s">
         <v>15</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="U2" s="9"/>
       <c r="V2" s="10"/>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="3" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="120" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1771,7 +1771,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
-      <c r="S3" s="116"/>
+      <c r="S3" s="103"/>
       <c r="T3" s="19"/>
       <c r="U3" s="20"/>
       <c r="V3" s="3"/>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="4" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="109"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="21" t="s">
         <v>20</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
       <c r="R4" s="24"/>
-      <c r="S4" s="117"/>
+      <c r="S4" s="104"/>
       <c r="T4" s="28"/>
       <c r="U4" s="20"/>
       <c r="V4" s="3"/>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="5" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="109"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="21" t="s">
         <v>23</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="P5" s="24"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
-      <c r="S5" s="117"/>
+      <c r="S5" s="104"/>
       <c r="T5" s="28"/>
       <c r="U5" s="20"/>
       <c r="V5" s="3"/>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="6" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="109"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="21" t="s">
         <v>26</v>
       </c>
@@ -1925,7 +1925,7 @@
       <c r="P6" s="24"/>
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
-      <c r="S6" s="117"/>
+      <c r="S6" s="104"/>
       <c r="T6" s="28"/>
       <c r="U6" s="20"/>
       <c r="V6" s="3"/>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="7" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="109"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="21" t="s">
         <v>30</v>
       </c>
@@ -1977,7 +1977,7 @@
       <c r="P7" s="24"/>
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
-      <c r="S7" s="117"/>
+      <c r="S7" s="104"/>
       <c r="T7" s="28"/>
       <c r="U7" s="20"/>
       <c r="V7" s="3"/>
@@ -2002,7 +2002,7 @@
     </row>
     <row r="8" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="109"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="21" t="s">
         <v>34</v>
       </c>
@@ -2029,7 +2029,7 @@
       <c r="P8" s="24"/>
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
-      <c r="S8" s="117"/>
+      <c r="S8" s="104"/>
       <c r="T8" s="28"/>
       <c r="U8" s="20"/>
       <c r="V8" s="3"/>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="9" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="109"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="21" t="s">
         <v>38</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
-      <c r="S9" s="117"/>
+      <c r="S9" s="104"/>
       <c r="T9" s="28"/>
       <c r="U9" s="20"/>
       <c r="V9" s="3"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="10" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="109"/>
+      <c r="B10" s="121"/>
       <c r="C10" s="21" t="s">
         <v>42</v>
       </c>
@@ -2133,7 +2133,7 @@
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
-      <c r="S10" s="117"/>
+      <c r="S10" s="104"/>
       <c r="T10" s="28"/>
       <c r="U10" s="20"/>
       <c r="V10" s="3"/>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="11" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="109"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="21" t="s">
         <v>46</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
-      <c r="S11" s="117"/>
+      <c r="S11" s="104"/>
       <c r="T11" s="28"/>
       <c r="U11" s="20"/>
       <c r="V11" s="3"/>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="12" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="109"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="21" t="s">
         <v>50</v>
       </c>
@@ -2237,7 +2237,7 @@
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
-      <c r="S12" s="117"/>
+      <c r="S12" s="104"/>
       <c r="T12" s="28"/>
       <c r="U12" s="20"/>
       <c r="V12" s="3"/>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="13" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="109"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="21" t="s">
         <v>54</v>
       </c>
@@ -2289,7 +2289,7 @@
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
-      <c r="S13" s="117"/>
+      <c r="S13" s="104"/>
       <c r="T13" s="28"/>
       <c r="U13" s="20"/>
       <c r="V13" s="3"/>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="14" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="110"/>
+      <c r="B14" s="122"/>
       <c r="C14" s="21" t="s">
         <v>58</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
-      <c r="S14" s="117"/>
+      <c r="S14" s="104"/>
       <c r="T14" s="28"/>
       <c r="U14" s="20"/>
       <c r="V14" s="3"/>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="15" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="123" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="32" t="s">
@@ -2391,7 +2391,7 @@
       <c r="P15" s="34"/>
       <c r="Q15" s="34"/>
       <c r="R15" s="34"/>
-      <c r="S15" s="118"/>
+      <c r="S15" s="105"/>
       <c r="T15" s="38"/>
       <c r="U15" s="20"/>
       <c r="V15" s="3"/>
@@ -2416,18 +2416,18 @@
     </row>
     <row r="16" spans="1:40" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="109"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="39" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" s="42"/>
       <c r="H16" s="43"/>
@@ -2441,7 +2441,7 @@
       <c r="P16" s="44"/>
       <c r="Q16" s="44"/>
       <c r="R16" s="44"/>
-      <c r="S16" s="118"/>
+      <c r="S16" s="105"/>
       <c r="T16" s="38"/>
       <c r="U16" s="20"/>
       <c r="V16" s="3"/>
@@ -2466,18 +2466,18 @@
     </row>
     <row r="17" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="109"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="46" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G17" s="42"/>
       <c r="H17" s="47"/>
@@ -2491,7 +2491,7 @@
       <c r="P17" s="48"/>
       <c r="Q17" s="48"/>
       <c r="R17" s="48"/>
-      <c r="S17" s="118"/>
+      <c r="S17" s="105"/>
       <c r="T17" s="50"/>
       <c r="U17" s="20"/>
       <c r="V17" s="3"/>
@@ -2516,16 +2516,16 @@
     </row>
     <row r="18" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="109"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="46" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="41" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G18" s="42"/>
       <c r="H18" s="51"/>
@@ -2539,7 +2539,7 @@
       <c r="P18" s="41"/>
       <c r="Q18" s="41"/>
       <c r="R18" s="41"/>
-      <c r="S18" s="119"/>
+      <c r="S18" s="106"/>
       <c r="T18" s="50"/>
       <c r="U18" s="20"/>
       <c r="V18" s="3"/>
@@ -2564,18 +2564,18 @@
     </row>
     <row r="19" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="109"/>
+      <c r="B19" s="121"/>
       <c r="C19" s="53" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G19" s="42"/>
       <c r="H19" s="51"/>
@@ -2589,7 +2589,7 @@
       <c r="P19" s="41"/>
       <c r="Q19" s="41"/>
       <c r="R19" s="41"/>
-      <c r="S19" s="119"/>
+      <c r="S19" s="106"/>
       <c r="T19" s="50"/>
       <c r="U19" s="20"/>
       <c r="V19" s="3"/>
@@ -2614,18 +2614,18 @@
     </row>
     <row r="20" spans="1:40" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="109"/>
+      <c r="B20" s="121"/>
       <c r="C20" s="53" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G20" s="42"/>
       <c r="H20" s="51"/>
@@ -2639,7 +2639,7 @@
       <c r="P20" s="41"/>
       <c r="Q20" s="41"/>
       <c r="R20" s="41"/>
-      <c r="S20" s="119"/>
+      <c r="S20" s="106"/>
       <c r="T20" s="50"/>
       <c r="U20" s="20"/>
       <c r="V20" s="3"/>
@@ -2664,18 +2664,18 @@
     </row>
     <row r="21" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="109"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="53" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G21" s="42"/>
       <c r="H21" s="51"/>
@@ -2689,7 +2689,7 @@
       <c r="P21" s="41"/>
       <c r="Q21" s="41"/>
       <c r="R21" s="41"/>
-      <c r="S21" s="119"/>
+      <c r="S21" s="106"/>
       <c r="T21" s="50"/>
       <c r="U21" s="20"/>
       <c r="V21" s="3"/>
@@ -2714,18 +2714,18 @@
     </row>
     <row r="22" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="110"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="54" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G22" s="57"/>
       <c r="H22" s="58"/>
@@ -2739,7 +2739,7 @@
       <c r="P22" s="56"/>
       <c r="Q22" s="56"/>
       <c r="R22" s="56"/>
-      <c r="S22" s="120"/>
+      <c r="S22" s="107"/>
       <c r="T22" s="60"/>
       <c r="U22" s="20"/>
       <c r="V22" s="3"/>
@@ -2764,17 +2764,17 @@
     </row>
     <row r="23" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="112" t="s">
-        <v>86</v>
+      <c r="B23" s="124" t="s">
+        <v>82</v>
       </c>
       <c r="C23" s="61" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E23" s="63" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F23" s="63" t="s">
         <v>22</v>
@@ -2791,7 +2791,7 @@
       <c r="P23" s="66"/>
       <c r="Q23" s="66"/>
       <c r="R23" s="63"/>
-      <c r="S23" s="121"/>
+      <c r="S23" s="108"/>
       <c r="T23" s="67"/>
       <c r="U23" s="20"/>
       <c r="V23" s="3"/>
@@ -2816,18 +2816,18 @@
     </row>
     <row r="24" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="109"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="68" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D24" s="69" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E24" s="70" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F24" s="70" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G24" s="71"/>
       <c r="H24" s="72"/>
@@ -2866,18 +2866,18 @@
     </row>
     <row r="25" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="110"/>
+      <c r="B25" s="122"/>
       <c r="C25" s="75" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D25" s="76" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="E25" s="77" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F25" s="77" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G25" s="78"/>
       <c r="H25" s="79"/>
@@ -2891,7 +2891,7 @@
       <c r="P25" s="77"/>
       <c r="Q25" s="77"/>
       <c r="R25" s="80"/>
-      <c r="S25" s="122"/>
+      <c r="S25" s="109"/>
       <c r="T25" s="81"/>
       <c r="U25" s="20"/>
       <c r="V25" s="3"/>
@@ -2916,17 +2916,17 @@
     </row>
     <row r="26" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="113" t="s">
-        <v>95</v>
+      <c r="B26" s="125" t="s">
+        <v>90</v>
       </c>
       <c r="C26" s="82" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D26" s="83" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E26" s="84" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F26" s="84" t="s">
         <v>22</v>
@@ -2943,7 +2943,7 @@
       <c r="P26" s="87"/>
       <c r="Q26" s="87"/>
       <c r="R26" s="87"/>
-      <c r="S26" s="123"/>
+      <c r="S26" s="110"/>
       <c r="T26" s="88"/>
       <c r="U26" s="20"/>
       <c r="V26" s="3"/>
@@ -2968,15 +2968,15 @@
     </row>
     <row r="27" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="109"/>
+      <c r="B27" s="121"/>
       <c r="C27" s="82" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D27" s="89" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E27" s="90" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F27" s="90" t="s">
         <v>19</v>
@@ -2993,8 +2993,8 @@
       <c r="P27" s="84"/>
       <c r="Q27" s="84"/>
       <c r="R27" s="84"/>
-      <c r="S27" s="123"/>
-      <c r="T27" s="125"/>
+      <c r="S27" s="110"/>
+      <c r="T27" s="112"/>
       <c r="U27" s="20"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
@@ -3018,18 +3018,18 @@
     </row>
     <row r="28" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="110"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="93" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D28" s="94" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E28" s="95" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F28" s="96" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G28" s="97"/>
       <c r="H28" s="98"/>
@@ -3085,7 +3085,7 @@
       <c r="P29" s="100"/>
       <c r="Q29" s="100"/>
       <c r="R29" s="100"/>
-      <c r="S29" s="124"/>
+      <c r="S29" s="111"/>
       <c r="T29" s="100"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
@@ -3127,7 +3127,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
-      <c r="S30" s="124"/>
+      <c r="S30" s="111"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
@@ -3169,7 +3169,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
-      <c r="S31" s="124"/>
+      <c r="S31" s="111"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
@@ -3211,7 +3211,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
-      <c r="S32" s="124"/>
+      <c r="S32" s="111"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
@@ -3253,7 +3253,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
-      <c r="S33" s="124"/>
+      <c r="S33" s="111"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
@@ -3295,7 +3295,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
-      <c r="S34" s="124"/>
+      <c r="S34" s="111"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="35" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="102"/>
+      <c r="B35" s="113"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -3337,7 +3337,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
-      <c r="S35" s="124"/>
+      <c r="S35" s="111"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="36" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="103"/>
+      <c r="B36" s="114"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -3379,7 +3379,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="124"/>
+      <c r="S36" s="111"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
@@ -3404,7 +3404,7 @@
     </row>
     <row r="37" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="103"/>
+      <c r="B37" s="114"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -3421,7 +3421,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="124"/>
+      <c r="S37" s="111"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="38" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="103"/>
+      <c r="B38" s="114"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -3463,7 +3463,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="124"/>
+      <c r="S38" s="111"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="39" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="103"/>
+      <c r="B39" s="114"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -3505,7 +3505,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="124"/>
+      <c r="S39" s="111"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="40" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="103"/>
+      <c r="B40" s="114"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -3547,7 +3547,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="124"/>
+      <c r="S40" s="111"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="41" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="103"/>
+      <c r="B41" s="114"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -3589,7 +3589,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="124"/>
+      <c r="S41" s="111"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
@@ -3614,7 +3614,7 @@
     </row>
     <row r="42" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="104"/>
+      <c r="B42" s="115"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -3631,7 +3631,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="124"/>
+      <c r="S42" s="111"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="43" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="102"/>
+      <c r="B43" s="113"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -3673,7 +3673,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="124"/>
+      <c r="S43" s="111"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
@@ -3698,7 +3698,7 @@
     </row>
     <row r="44" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="103"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -3715,7 +3715,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-      <c r="S44" s="124"/>
+      <c r="S44" s="111"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
@@ -3740,7 +3740,7 @@
     </row>
     <row r="45" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="103"/>
+      <c r="B45" s="114"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -3757,7 +3757,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
-      <c r="S45" s="124"/>
+      <c r="S45" s="111"/>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
@@ -3782,7 +3782,7 @@
     </row>
     <row r="46" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="103"/>
+      <c r="B46" s="114"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -3799,7 +3799,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="124"/>
+      <c r="S46" s="111"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="47" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="104"/>
+      <c r="B47" s="115"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -3841,7 +3841,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
-      <c r="S47" s="124"/>
+      <c r="S47" s="111"/>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="48" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="102"/>
+      <c r="B48" s="113"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -3883,7 +3883,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
-      <c r="S48" s="124"/>
+      <c r="S48" s="111"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
@@ -3908,7 +3908,7 @@
     </row>
     <row r="49" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="103"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -3925,7 +3925,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
-      <c r="S49" s="124"/>
+      <c r="S49" s="111"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="50" spans="1:40" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="104"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -3967,7 +3967,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
-      <c r="S50" s="124"/>
+      <c r="S50" s="111"/>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
@@ -4009,7 +4009,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
-      <c r="S51" s="124"/>
+      <c r="S51" s="111"/>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
       <c r="V51" s="1"/>
@@ -4051,7 +4051,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
-      <c r="S52" s="124"/>
+      <c r="S52" s="111"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
@@ -4093,7 +4093,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
-      <c r="S53" s="124"/>
+      <c r="S53" s="111"/>
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
@@ -4135,7 +4135,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
-      <c r="S54" s="124"/>
+      <c r="S54" s="111"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
@@ -4177,7 +4177,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
-      <c r="S55" s="124"/>
+      <c r="S55" s="111"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
@@ -4219,7 +4219,7 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
-      <c r="S56" s="124"/>
+      <c r="S56" s="111"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
@@ -4261,7 +4261,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
-      <c r="S57" s="124"/>
+      <c r="S57" s="111"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
@@ -4303,7 +4303,7 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
-      <c r="S58" s="124"/>
+      <c r="S58" s="111"/>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
@@ -4345,7 +4345,7 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
-      <c r="S59" s="124"/>
+      <c r="S59" s="111"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
@@ -4387,7 +4387,7 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
-      <c r="S60" s="124"/>
+      <c r="S60" s="111"/>
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
@@ -4429,7 +4429,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
-      <c r="S61" s="124"/>
+      <c r="S61" s="111"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
@@ -4471,7 +4471,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
-      <c r="S62" s="124"/>
+      <c r="S62" s="111"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
@@ -4513,7 +4513,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
-      <c r="S63" s="124"/>
+      <c r="S63" s="111"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
@@ -4555,7 +4555,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
-      <c r="S64" s="124"/>
+      <c r="S64" s="111"/>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
       <c r="V64" s="1"/>
@@ -4597,7 +4597,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
-      <c r="S65" s="124"/>
+      <c r="S65" s="111"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
@@ -4639,7 +4639,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
-      <c r="S66" s="124"/>
+      <c r="S66" s="111"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
       <c r="V66" s="1"/>
@@ -4681,7 +4681,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
-      <c r="S67" s="124"/>
+      <c r="S67" s="111"/>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
@@ -4723,7 +4723,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
-      <c r="S68" s="124"/>
+      <c r="S68" s="111"/>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
@@ -4765,7 +4765,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
-      <c r="S69" s="124"/>
+      <c r="S69" s="111"/>
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
@@ -4807,7 +4807,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
-      <c r="S70" s="124"/>
+      <c r="S70" s="111"/>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
@@ -4849,7 +4849,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
-      <c r="S71" s="124"/>
+      <c r="S71" s="111"/>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
@@ -4891,7 +4891,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
-      <c r="S72" s="124"/>
+      <c r="S72" s="111"/>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
@@ -4933,7 +4933,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
-      <c r="S73" s="124"/>
+      <c r="S73" s="111"/>
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
@@ -4975,7 +4975,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
-      <c r="S74" s="124"/>
+      <c r="S74" s="111"/>
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
@@ -5017,7 +5017,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
-      <c r="S75" s="124"/>
+      <c r="S75" s="111"/>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
@@ -5059,7 +5059,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
-      <c r="S76" s="124"/>
+      <c r="S76" s="111"/>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
@@ -44032,6 +44032,6 @@
     <hyperlink ref="E28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>